<commit_message>
change column names in excel
for better workflow in R
</commit_message>
<xml_diff>
--- a/data/processed/Example_Indicators/Ausweichdistanz_example.xlsx
+++ b/data/processed/Example_Indicators/Ausweichdistanz_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\am17w286\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\am17w286\Documents\GitHub\Projekt_Antibiotikaverbrauch\data\processed\Example_Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CADF92-0181-4338-8F8A-5359EF41A32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840F71DD-6D4D-48D8-BBC7-8CDCFBA2B662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,18 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>0-50</t>
-  </si>
-  <si>
-    <t>50-100</t>
-  </si>
-  <si>
-    <t>&gt;100</t>
   </si>
   <si>
     <t>AMU</t>
@@ -60,6 +51,18 @@
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>touch</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>far</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -441,25 +444,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
-        <v>0</v>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -467,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>99.999999999999986</v>
@@ -490,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -513,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -536,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>99.999999999999986</v>
@@ -559,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -582,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -605,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>99.999999999999986</v>
@@ -628,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -651,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -674,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>99.999999999999986</v>
@@ -697,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -720,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -743,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -766,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -789,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -812,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>100.00000000000001</v>
@@ -835,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>100.00000000000001</v>
@@ -858,7 +861,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -881,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -904,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>99.999999999999986</v>
@@ -927,7 +930,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -950,7 +953,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>100.00000000000001</v>
@@ -973,7 +976,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -996,7 +999,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -1019,7 +1022,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -1042,7 +1045,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>99.999999999999986</v>
@@ -1065,7 +1068,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>100</v>
@@ -1088,7 +1091,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>100.00000000000001</v>
@@ -1111,7 +1114,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -1134,7 +1137,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>99.999999999999986</v>
@@ -1157,7 +1160,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1180,7 +1183,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1203,7 +1206,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>99.999999999999986</v>
@@ -1226,7 +1229,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1249,7 +1252,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>99.999999999999986</v>
@@ -1272,7 +1275,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <v>99.999999999999986</v>
@@ -1295,7 +1298,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>100</v>
@@ -1318,7 +1321,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>100</v>
@@ -1341,7 +1344,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -1364,7 +1367,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -1387,7 +1390,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>99.999999999999986</v>
@@ -1410,7 +1413,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1433,7 +1436,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1456,7 +1459,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1479,7 +1482,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>99.999999999999986</v>
@@ -1502,7 +1505,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>100.00000000000001</v>
@@ -1525,7 +1528,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>100</v>
@@ -1548,7 +1551,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>100</v>
@@ -1571,7 +1574,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -1594,7 +1597,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>100</v>

</xml_diff>